<commit_message>
modidy docs and readme
</commit_message>
<xml_diff>
--- a/docs/入力データ作成例.xlsx
+++ b/docs/入力データ作成例.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ec0b57064cda302b/Desktop/PriCre/Link_Simulator/main/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onishilab-my.sharepoint.com/personal/takuya_takase_onishilab_onmicrosoft_com/Documents/デスクトップ/就活/ポートフォリオ用資料/link_simulator/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="11_AD4D066CA252ABDACC1048AAA191CBF873EEDF51" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E19E01D-1973-4151-90F2-50CAE958EC84}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="11_AD4D066CA252ABDACC1048AAA191CBF873EEDF51" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF92745F-F9E8-4EB8-BE59-D77A3567FCE7}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="with説明" sheetId="1" r:id="rId1"/>
@@ -191,7 +191,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,29 +215,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Yu Gothic"/>
-      <family val="3"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
-      <name val="Yu Gothic"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Yu Gothic"/>
-      <family val="3"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF00B050"/>
       <name val="Yu Gothic"/>
       <family val="2"/>
@@ -248,6 +225,38 @@
       <color theme="4"/>
       <name val="Yu Gothic"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Yu Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -307,41 +316,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -357,22 +367,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person0.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
-<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -638,332 +632,335 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="12.125" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.75" customWidth="1"/>
-    <col min="5" max="5" width="4.4140625" customWidth="1"/>
-    <col min="8" max="8" width="62.9140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.08203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="2.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.75" customWidth="1"/>
+    <col min="7" max="7" width="57.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="H1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="7">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7">
-        <v>0</v>
-      </c>
-      <c r="C2" s="9">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="G1" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="5">
         <v>3</v>
       </c>
-      <c r="E2" s="13">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="7">
+    <row r="3" spans="1:7">
+      <c r="A3" s="3">
         <v>-38</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="3">
         <v>-7.8</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="11">
-        <v>0</v>
-      </c>
-      <c r="E3" s="13"/>
-      <c r="H3" s="6" t="s">
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="G3" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="7">
-        <v>0</v>
-      </c>
-      <c r="B4" s="7">
-        <v>0</v>
-      </c>
-      <c r="C4" s="9">
-        <v>0</v>
-      </c>
-      <c r="D4" s="11">
-        <v>0</v>
-      </c>
-      <c r="E4" s="13"/>
-      <c r="H4" s="8" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4" s="3">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="G4" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="7">
-        <v>0</v>
-      </c>
-      <c r="B5" s="7">
-        <v>0</v>
-      </c>
-      <c r="C5" s="9">
-        <v>0</v>
-      </c>
-      <c r="D5" s="11">
-        <v>0</v>
-      </c>
-      <c r="E5" s="13"/>
-      <c r="H5" s="10" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" s="3">
+        <v>0</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="G5" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="7">
-        <v>0</v>
-      </c>
-      <c r="B6" s="7">
-        <v>0</v>
-      </c>
-      <c r="C6" s="9">
-        <v>0</v>
-      </c>
-      <c r="D6" s="11">
-        <v>0</v>
-      </c>
-      <c r="E6" s="13"/>
-      <c r="H6" s="12" t="s">
+    <row r="6" spans="1:7">
+      <c r="A6" s="3">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="G6" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="7">
-        <v>0</v>
-      </c>
-      <c r="B7" s="7">
-        <v>0</v>
-      </c>
-      <c r="C7" s="9">
-        <v>0</v>
-      </c>
-      <c r="D7" s="11">
-        <v>0</v>
-      </c>
-      <c r="E7" s="13"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="7">
-        <v>0</v>
-      </c>
-      <c r="B8" s="7">
-        <v>0</v>
-      </c>
-      <c r="C8" s="9">
-        <v>0</v>
-      </c>
-      <c r="D8" s="11">
-        <v>0</v>
-      </c>
-      <c r="E8" s="13"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="7">
-        <v>0</v>
-      </c>
-      <c r="B9" s="7">
-        <v>0</v>
-      </c>
-      <c r="C9" s="9">
-        <v>0</v>
-      </c>
-      <c r="D9" s="11">
-        <v>0</v>
-      </c>
-      <c r="E9" s="13"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="16">
+    <row r="7" spans="1:7">
+      <c r="A7" s="3">
+        <v>0</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="3">
+        <v>0</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="3">
+        <v>0</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="7">
         <v>1</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="7">
         <v>3</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="8">
         <v>15</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="H10" s="3" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="G10" s="16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="16">
+    <row r="11" spans="1:7">
+      <c r="A11" s="7">
         <v>2</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="7">
         <v>4</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="8">
         <v>41.5</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="H11" s="14" t="s">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="G11" s="17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="16">
+    <row r="12" spans="1:7">
+      <c r="A12" s="7">
         <v>2</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="7">
         <v>5</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="8">
         <v>40.1</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="H12" s="15" t="s">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="G12" s="18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="16">
+    <row r="13" spans="1:7">
+      <c r="A13" s="7">
         <v>2</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="7">
         <v>6</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="8">
         <v>39.299999999999997</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="H13" t="s">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="G13" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="16">
+    <row r="14" spans="1:7">
+      <c r="A14" s="7">
         <v>3</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="7">
         <v>4</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="8">
         <v>50</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="16">
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="7">
         <v>3</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="7">
         <v>6</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="8">
         <v>61.5</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="16">
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="7">
         <v>4</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="7">
         <v>5</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="8">
         <v>55.8</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="16">
+      <c r="A17" s="7">
         <v>5</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="7">
         <v>7</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="8">
         <v>39.4</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="16">
+      <c r="A18" s="7">
         <v>6</v>
       </c>
-      <c r="B18" s="16">
+      <c r="B18" s="7">
         <v>7</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="8">
         <v>36.700000000000003</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="16">
+      <c r="A19" s="7">
         <v>6</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="7">
         <v>8</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="8">
         <v>49</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="16">
+      <c r="A20" s="7">
         <v>7</v>
       </c>
-      <c r="B20" s="16">
+      <c r="B20" s="7">
         <v>8</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="8">
         <v>65.7</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>